<commit_message>
fixed printing free air space
</commit_message>
<xml_diff>
--- a/Test Basic Pull Sheet.xlsx
+++ b/Test Basic Pull Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roneill\Documents\CRO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7D0127-01EF-4F73-A1EA-40A0969F9ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D2D79F-04C4-40AF-872B-9006CC412103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31530" yWindow="2670" windowWidth="12150" windowHeight="20835" xr2:uid="{B55DDC81-D8A6-4AC8-B7A6-3CDB36520BB6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>Pull #</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>12C#14</t>
-  </si>
-  <si>
-    <t>CABLE 1</t>
   </si>
 </sst>
 </file>
@@ -838,33 +835,14 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="4">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>

</xml_diff>

<commit_message>
Sort stationing + size
</commit_message>
<xml_diff>
--- a/Test Basic Pull Sheet.xlsx
+++ b/Test Basic Pull Sheet.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://judlauent-my.sharepoint.com/personal/roneill_tcelect_net/Documents/Documents 1/Code/Git Files/Cable-Run-Optimizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{D77271E0-B3CA-4731-BF91-1E71098F0430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98714EE6-8A58-45C3-9085-C1E1A9419AFB}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{D77271E0-B3CA-4731-BF91-1E71098F0430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{204D9D92-68E5-48D8-9C9E-DE4EB08A5480}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{B55DDC81-D8A6-4AC8-B7A6-3CDB36520BB6}"/>
+    <workbookView xWindow="15" yWindow="300" windowWidth="13785" windowHeight="15075" xr2:uid="{B55DDC81-D8A6-4AC8-B7A6-3CDB36520BB6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2.1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="19">
   <si>
     <t>Pull #</t>
   </si>
@@ -90,6 +91,9 @@
   </si>
   <si>
     <t>10C#14</t>
+  </si>
+  <si>
+    <t>12C#14</t>
   </si>
 </sst>
 </file>
@@ -646,10 +650,489 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{201A0316-6B2F-4DAF-B941-AD7334AF299B}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C54F67-24E4-4C2A-B4B7-7439936B8FDB}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cable Sizing + Iterating Properly
</commit_message>
<xml_diff>
--- a/Test Basic Pull Sheet.xlsx
+++ b/Test Basic Pull Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://judlauent-my.sharepoint.com/personal/roneill_tcelect_net/Documents/Documents 1/Code/Git Files/Cable-Run-Optimizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{D77271E0-B3CA-4731-BF91-1E71098F0430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDAC6DB6-68D2-4182-AD42-9F58268CF44E}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{D77271E0-B3CA-4731-BF91-1E71098F0430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE276F95-642B-4D55-8C9F-48EFD8D3FA6A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B55DDC81-D8A6-4AC8-B7A6-3CDB36520BB6}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="21">
   <si>
     <t>Pull #</t>
   </si>
@@ -651,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{201A0316-6B2F-4DAF-B941-AD7334AF299B}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +690,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -699,7 +699,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -728,7 +728,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -748,7 +748,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -757,7 +757,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -777,7 +777,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -806,7 +806,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -835,7 +835,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -888,412 +888,6 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="F12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-      <c r="F14" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="F15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
-      <c r="F16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
         <v>0</v>
       </c>
     </row>
@@ -1304,10 +898,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C54F67-24E4-4C2A-B4B7-7439936B8FDB}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:F7"/>
+    <sheetView topLeftCell="A21" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,6 +1075,615 @@
       </c>
       <c r="F7" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" t="s">
+        <v>10</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed inner cable remove
</commit_message>
<xml_diff>
--- a/Test Basic Pull Sheet.xlsx
+++ b/Test Basic Pull Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://judlauent-my.sharepoint.com/personal/roneill_tcelect_net/Documents/Documents 1/Code/Git Files/Cable-Run-Optimizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{D23D06AD-18E3-4183-AC80-8894A5B21212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A7FB1AA-7BB1-4B08-9BD8-6DBBED81645E}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{D23D06AD-18E3-4183-AC80-8894A5B21212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5B16E0C-C32B-4CC1-B2DF-1F37C4B1C0B3}"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="450" windowWidth="18015" windowHeight="14205" xr2:uid="{B55DDC81-D8A6-4AC8-B7A6-3CDB36520BB6}"/>
+    <workbookView xWindow="3990" yWindow="870" windowWidth="19695" windowHeight="14205" xr2:uid="{B55DDC81-D8A6-4AC8-B7A6-3CDB36520BB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="23">
   <si>
     <t>Pull #</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>EXPRESS</t>
+  </si>
+  <si>
+    <t>500+00</t>
+  </si>
+  <si>
+    <t>600+00</t>
+  </si>
+  <si>
+    <t>STAR QUAD</t>
+  </si>
+  <si>
+    <t>2C#6</t>
   </si>
 </sst>
 </file>
@@ -146,6 +158,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -445,13 +461,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{201A0316-6B2F-4DAF-B941-AD7334AF299B}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1117,6 +1136,238 @@
         <v>0</v>
       </c>
       <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Stationing Parsing Logic
</commit_message>
<xml_diff>
--- a/Test Basic Pull Sheet.xlsx
+++ b/Test Basic Pull Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://judlauent-my.sharepoint.com/personal/roneill_tcelect_net/Documents/Documents 1/Code/Git Files/Cable-Run-Optimizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{D23D06AD-18E3-4183-AC80-8894A5B21212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{817BB89A-3316-41E4-BE66-B99D4C74167D}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="13_ncr:1_{D23D06AD-18E3-4183-AC80-8894A5B21212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1C4F916-4FBC-494A-B507-5422E942489E}"/>
   <bookViews>
-    <workbookView xWindow="17805" yWindow="825" windowWidth="10410" windowHeight="10560" xr2:uid="{B55DDC81-D8A6-4AC8-B7A6-3CDB36520BB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B55DDC81-D8A6-4AC8-B7A6-3CDB36520BB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -467,7 +467,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +629,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="I8" sqref="I8:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Sorting Cables by Shorter Ones Dropping Out First
</commit_message>
<xml_diff>
--- a/Test Basic Pull Sheet.xlsx
+++ b/Test Basic Pull Sheet.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://judlauent-my.sharepoint.com/personal/roneill_tcelect_net/Documents/Documents 1/Code/Git Files/Cable-Run-Optimizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="241" documentId="13_ncr:1_{D23D06AD-18E3-4183-AC80-8894A5B21212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9474BD5A-4CC6-4209-9ECA-38B7AD7AEB03}"/>
+  <xr:revisionPtr revIDLastSave="294" documentId="13_ncr:1_{D23D06AD-18E3-4183-AC80-8894A5B21212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8162D46-9035-42DD-BA22-9950FC781F0C}"/>
   <bookViews>
-    <workbookView xWindow="9450" yWindow="270" windowWidth="19005" windowHeight="14385" xr2:uid="{B55DDC81-D8A6-4AC8-B7A6-3CDB36520BB6}"/>
+    <workbookView xWindow="9945" yWindow="1710" windowWidth="14880" windowHeight="12150" xr2:uid="{B55DDC81-D8A6-4AC8-B7A6-3CDB36520BB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="27">
   <si>
     <t>Pull #</t>
   </si>
@@ -104,6 +105,21 @@
   </si>
   <si>
     <t>3C#9</t>
+  </si>
+  <si>
+    <t>1C#4</t>
+  </si>
+  <si>
+    <t>200+00</t>
+  </si>
+  <si>
+    <t>300+00</t>
+  </si>
+  <si>
+    <t>400+00</t>
+  </si>
+  <si>
+    <t>7C#10</t>
   </si>
 </sst>
 </file>
@@ -468,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{201A0316-6B2F-4DAF-B941-AD7334AF299B}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,16 +523,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -524,16 +540,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -541,16 +557,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -558,543 +574,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" t="s">
-        <v>2</v>
-      </c>
-      <c r="E24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
         <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" t="s">
-        <v>2</v>
-      </c>
-      <c r="E26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" t="s">
-        <v>2</v>
-      </c>
-      <c r="E27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" t="s">
-        <v>2</v>
-      </c>
-      <c r="E29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" t="s">
-        <v>2</v>
-      </c>
-      <c r="E30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" t="s">
-        <v>2</v>
-      </c>
-      <c r="E32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" t="s">
-        <v>2</v>
-      </c>
-      <c r="E33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" t="s">
-        <v>2</v>
-      </c>
-      <c r="E34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" t="s">
-        <v>2</v>
-      </c>
-      <c r="E35" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" t="s">
-        <v>2</v>
-      </c>
-      <c r="E36" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1104,6 +593,786 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABA7D865-4FB5-41B9-A95D-CC32F1496B92}">
+  <dimension ref="A1:E45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" t="s">
+        <v>2</v>
+      </c>
+      <c r="E41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5F9924-AA7D-49DB-85CC-CC30A665294A}">
   <dimension ref="A1:F31"/>
   <sheetViews>
@@ -1648,7 +1917,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B880C181-07DD-4449-8445-7AAA5EB18EDD}">
   <dimension ref="A1:F39"/>
   <sheetViews>

</xml_diff>